<commit_message>
University - Program - Import data : Start dates not exist in excel sheet
</commit_message>
<xml_diff>
--- a/backend/web/samples/Universitie-Programs.xlsx
+++ b/backend/web/samples/Universitie-Programs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23023"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23107"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{75DC4D13-6545-404D-B55D-E15BEFD54026}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{19F87F0C-5D3B-424E-838B-890BC7E72477}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191028" calcCompleted="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="72">
   <si>
     <t>Program Name</t>
   </si>
@@ -114,6 +114,9 @@
     <t>ملاحظات ٢</t>
   </si>
   <si>
+    <t>Start Dates</t>
+  </si>
+  <si>
     <t>Program one</t>
   </si>
   <si>
@@ -138,6 +141,9 @@
     <t>Day</t>
   </si>
   <si>
+    <t>yes</t>
+  </si>
+  <si>
     <t>YES</t>
   </si>
   <si>
@@ -177,6 +183,9 @@
     <t>ملاحظات ٢ ١</t>
   </si>
   <si>
+    <t>JAN,FEB,MAR,APR</t>
+  </si>
+  <si>
     <t>Program two</t>
   </si>
   <si>
@@ -232,6 +241,9 @@
   </si>
   <si>
     <t>ملاحظات ٢ ٢</t>
+  </si>
+  <si>
+    <t>JAN,FEB,MAR,APR,MAY,JUN,JUL,AUG</t>
   </si>
 </sst>
 </file>
@@ -612,10 +624,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AB3"/>
+  <dimension ref="A1:AC3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AD7" sqref="AD7"/>
+    <sheetView tabSelected="1" topLeftCell="W1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AB13" sqref="AB13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
@@ -641,10 +653,12 @@
     <col min="21" max="21" width="22.28515625" customWidth="1"/>
     <col min="22" max="22" width="19.85546875" customWidth="1"/>
     <col min="23" max="24" width="27.140625" customWidth="1"/>
-    <col min="25" max="67" width="9.140625"/>
+    <col min="25" max="28" width="9.140625"/>
+    <col min="29" max="29" width="19.5703125" customWidth="1"/>
+    <col min="30" max="67" width="9.140625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="1" customFormat="1">
+    <row r="1" spans="1:29" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -729,58 +743,61 @@
       <c r="AB1" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="AC1" s="1" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="2" spans="1:28">
+    <row r="2" spans="1:29">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H2">
         <v>2</v>
       </c>
       <c r="I2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="J2" s="3">
         <v>44036</v>
       </c>
       <c r="K2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="L2" s="3">
         <v>44128</v>
       </c>
       <c r="M2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="N2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="O2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="P2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="Q2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="R2">
         <v>5000</v>
@@ -792,81 +809,84 @@
         <v>150</v>
       </c>
       <c r="U2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="V2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="W2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="X2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="Y2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="Z2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="AA2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="AB2" t="s">
-        <v>48</v>
+        <v>50</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:28">
+    <row r="3" spans="1:29">
       <c r="A3" s="4" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B3" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C3" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="D3" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="E3" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="F3" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="G3" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="H3">
         <v>1</v>
       </c>
       <c r="I3" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="J3" s="3">
         <v>44098</v>
       </c>
       <c r="K3" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="L3" s="3">
         <v>44189</v>
       </c>
       <c r="M3" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="N3" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="O3" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="P3" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="Q3" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="R3">
         <v>1000</v>
@@ -878,28 +898,31 @@
         <v>60</v>
       </c>
       <c r="U3" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="V3" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="W3" s="5" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="X3" s="5" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="Y3" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="Z3" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="AA3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="AB3" t="s">
-        <v>67</v>
+        <v>70</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>